<commit_message>
97% progress, bugs: delete & moving hubkel
</commit_message>
<xml_diff>
--- a/db/data harlep otani.xlsx
+++ b/db/data harlep otani.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\hcmotani\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFEC5211-1700-4BB2-B005-5E16EFC005A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78400B60-C5C7-4ED4-AA7B-4118BA4811C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data sp" sheetId="1" r:id="rId1"/>
@@ -6449,22 +6449,22 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.140625" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="60.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="60.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="8"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -6472,7 +6472,7 @@
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -6492,7 +6492,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -6512,7 +6512,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>2</v>
       </c>
@@ -6532,7 +6532,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>3</v>
       </c>
@@ -6552,7 +6552,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>4</v>
       </c>
@@ -6572,7 +6572,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>5</v>
       </c>
@@ -6592,7 +6592,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>6</v>
       </c>
@@ -6625,33 +6625,33 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="5" width="34.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" ht="25.2" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
         <v>22</v>
       </c>
       <c r="K1" s="11"/>
       <c r="L1" s="11"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="K2" s="11"/>
       <c r="L2" s="11"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="42" t="s">
         <v>1</v>
       </c>
@@ -6689,7 +6689,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="43"/>
       <c r="B4" s="43"/>
       <c r="C4" s="43"/>
@@ -6711,7 +6711,7 @@
       </c>
       <c r="L4" s="41"/>
     </row>
-    <row r="5" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="5" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A5" s="15" t="s">
         <v>38</v>
       </c>
@@ -6747,7 +6747,7 @@
       </c>
       <c r="L5" s="18"/>
     </row>
-    <row r="6" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="6" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A6" s="15" t="s">
         <v>49</v>
       </c>
@@ -6783,7 +6783,7 @@
       </c>
       <c r="L6" s="18"/>
     </row>
-    <row r="7" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="7" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A7" s="15" t="s">
         <v>59</v>
       </c>
@@ -6821,7 +6821,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="8" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A8" s="15" t="s">
         <v>67</v>
       </c>
@@ -6859,7 +6859,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="9" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A9" s="15" t="s">
         <v>77</v>
       </c>
@@ -6895,7 +6895,7 @@
       </c>
       <c r="L9" s="18"/>
     </row>
-    <row r="10" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="10" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A10" s="15" t="s">
         <v>84</v>
       </c>
@@ -6933,7 +6933,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="11" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A11" s="15" t="s">
         <v>93</v>
       </c>
@@ -6969,7 +6969,7 @@
       </c>
       <c r="L11" s="18"/>
     </row>
-    <row r="12" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="12" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A12" s="15" t="s">
         <v>101</v>
       </c>
@@ -7005,7 +7005,7 @@
       </c>
       <c r="L12" s="18"/>
     </row>
-    <row r="13" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="13" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A13" s="15" t="s">
         <v>109</v>
       </c>
@@ -7033,7 +7033,7 @@
       <c r="K13" s="18"/>
       <c r="L13" s="18"/>
     </row>
-    <row r="14" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="14" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A14" s="15" t="s">
         <v>114</v>
       </c>
@@ -7071,7 +7071,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="15" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A15" s="15" t="s">
         <v>123</v>
       </c>
@@ -7109,7 +7109,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="16" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A16" s="15" t="s">
         <v>132</v>
       </c>
@@ -7147,7 +7147,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="17" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A17" s="15" t="s">
         <v>140</v>
       </c>
@@ -7185,7 +7185,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="18" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A18" s="15" t="s">
         <v>149</v>
       </c>
@@ -7223,7 +7223,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="19" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A19" s="15" t="s">
         <v>157</v>
       </c>
@@ -7261,7 +7261,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="20" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A20" s="15" t="s">
         <v>166</v>
       </c>
@@ -7299,7 +7299,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="21" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A21" s="15" t="s">
         <v>175</v>
       </c>
@@ -7335,7 +7335,7 @@
       </c>
       <c r="L21" s="18"/>
     </row>
-    <row r="22" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="22" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A22" s="15" t="s">
         <v>183</v>
       </c>
@@ -7371,7 +7371,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="23" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A23" s="15" t="s">
         <v>190</v>
       </c>
@@ -7407,7 +7407,7 @@
       </c>
       <c r="L23" s="18"/>
     </row>
-    <row r="24" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="24" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A24" s="15" t="s">
         <v>198</v>
       </c>
@@ -7443,7 +7443,7 @@
       </c>
       <c r="L24" s="25"/>
     </row>
-    <row r="25" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="25" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A25" s="15" t="s">
         <v>206</v>
       </c>
@@ -7481,7 +7481,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="26" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A26" s="15" t="s">
         <v>213</v>
       </c>
@@ -7517,7 +7517,7 @@
       </c>
       <c r="L26" s="25"/>
     </row>
-    <row r="27" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="27" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A27" s="15" t="s">
         <v>221</v>
       </c>
@@ -7553,7 +7553,7 @@
       </c>
       <c r="L27" s="25"/>
     </row>
-    <row r="28" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="28" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A28" s="15" t="s">
         <v>228</v>
       </c>
@@ -7587,7 +7587,7 @@
       </c>
       <c r="L28" s="25"/>
     </row>
-    <row r="29" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="29" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A29" s="15" t="s">
         <v>235</v>
       </c>
@@ -7623,7 +7623,7 @@
       </c>
       <c r="L29" s="25"/>
     </row>
-    <row r="30" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="30" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A30" s="15" t="s">
         <v>242</v>
       </c>
@@ -7659,7 +7659,7 @@
       </c>
       <c r="L30" s="25"/>
     </row>
-    <row r="31" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="31" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A31" s="15" t="s">
         <v>249</v>
       </c>
@@ -7695,7 +7695,7 @@
       </c>
       <c r="L31" s="25"/>
     </row>
-    <row r="32" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="32" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A32" s="15" t="s">
         <v>256</v>
       </c>
@@ -7731,7 +7731,7 @@
       </c>
       <c r="L32" s="25"/>
     </row>
-    <row r="33" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="33" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A33" s="15" t="s">
         <v>263</v>
       </c>
@@ -7767,7 +7767,7 @@
       </c>
       <c r="L33" s="25"/>
     </row>
-    <row r="34" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="34" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A34" s="15" t="s">
         <v>270</v>
       </c>
@@ -7803,7 +7803,7 @@
       </c>
       <c r="L34" s="25"/>
     </row>
-    <row r="35" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="35" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A35" s="15" t="s">
         <v>277</v>
       </c>
@@ -7841,7 +7841,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="36" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A36" s="15" t="s">
         <v>284</v>
       </c>
@@ -7877,7 +7877,7 @@
       </c>
       <c r="L36" s="25"/>
     </row>
-    <row r="37" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="37" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A37" s="15" t="s">
         <v>292</v>
       </c>
@@ -7911,7 +7911,7 @@
       <c r="K37" s="25"/>
       <c r="L37" s="25"/>
     </row>
-    <row r="38" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="38" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A38" s="15" t="s">
         <v>299</v>
       </c>
@@ -7947,7 +7947,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="39" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A39" s="15" t="s">
         <v>307</v>
       </c>
@@ -7985,7 +7985,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="40" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A40" s="15" t="s">
         <v>316</v>
       </c>
@@ -8019,7 +8019,7 @@
       </c>
       <c r="L40" s="25"/>
     </row>
-    <row r="41" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="41" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A41" s="15" t="s">
         <v>322</v>
       </c>
@@ -8041,7 +8041,7 @@
       <c r="K41" s="18"/>
       <c r="L41" s="25"/>
     </row>
-    <row r="42" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="42" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A42" s="15" t="s">
         <v>324</v>
       </c>
@@ -8079,7 +8079,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="43" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A43" s="15" t="s">
         <v>334</v>
       </c>
@@ -8117,7 +8117,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="44" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A44" s="15" t="s">
         <v>343</v>
       </c>
@@ -8155,7 +8155,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="45" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A45" s="15" t="s">
         <v>353</v>
       </c>
@@ -8191,7 +8191,7 @@
       </c>
       <c r="L45" s="25"/>
     </row>
-    <row r="46" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="46" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A46" s="15" t="s">
         <v>361</v>
       </c>
@@ -8229,7 +8229,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="47" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A47" s="15" t="s">
         <v>370</v>
       </c>
@@ -8265,7 +8265,7 @@
       </c>
       <c r="L47" s="25"/>
     </row>
-    <row r="48" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="48" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A48" s="15" t="s">
         <v>336</v>
       </c>
@@ -8301,7 +8301,7 @@
       </c>
       <c r="L48" s="25"/>
     </row>
-    <row r="49" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="49" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A49" s="15" t="s">
         <v>385</v>
       </c>
@@ -8337,7 +8337,7 @@
       </c>
       <c r="L49" s="25"/>
     </row>
-    <row r="50" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="50" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A50" s="15" t="s">
         <v>393</v>
       </c>
@@ -8371,7 +8371,7 @@
       </c>
       <c r="L50" s="25"/>
     </row>
-    <row r="51" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="51" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A51" s="15" t="s">
         <v>399</v>
       </c>
@@ -8407,7 +8407,7 @@
       </c>
       <c r="L51" s="25"/>
     </row>
-    <row r="52" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="52" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A52" s="15" t="s">
         <v>407</v>
       </c>
@@ -8445,7 +8445,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="53" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A53" s="15" t="s">
         <v>416</v>
       </c>
@@ -8483,7 +8483,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="54" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A54" s="15" t="s">
         <v>423</v>
       </c>
@@ -8521,7 +8521,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="55" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A55" s="15" t="s">
         <v>431</v>
       </c>
@@ -8557,7 +8557,7 @@
       </c>
       <c r="L55" s="25"/>
     </row>
-    <row r="56" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="56" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A56" s="15" t="s">
         <v>438</v>
       </c>
@@ -8593,7 +8593,7 @@
       </c>
       <c r="L56" s="25"/>
     </row>
-    <row r="57" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="57" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A57" s="15" t="s">
         <v>445</v>
       </c>
@@ -8629,7 +8629,7 @@
       </c>
       <c r="L57" s="25"/>
     </row>
-    <row r="58" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="58" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A58" s="15" t="s">
         <v>451</v>
       </c>
@@ -8665,7 +8665,7 @@
       </c>
       <c r="L58" s="25"/>
     </row>
-    <row r="59" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="59" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A59" s="15" t="s">
         <v>456</v>
       </c>
@@ -8701,7 +8701,7 @@
       </c>
       <c r="L59" s="25"/>
     </row>
-    <row r="60" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="60" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A60" s="15" t="s">
         <v>462</v>
       </c>
@@ -8729,7 +8729,7 @@
       <c r="K60" s="18"/>
       <c r="L60" s="25"/>
     </row>
-    <row r="61" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="61" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A61" s="15" t="s">
         <v>467</v>
       </c>
@@ -8767,7 +8767,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="62" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A62" s="15" t="s">
         <v>475</v>
       </c>
@@ -8805,7 +8805,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="63" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A63" s="15" t="s">
         <v>483</v>
       </c>
@@ -8843,7 +8843,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="64" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A64" s="15" t="s">
         <v>491</v>
       </c>
@@ -8881,7 +8881,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="65" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A65" s="15" t="s">
         <v>499</v>
       </c>
@@ -8919,7 +8919,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="66" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A66" s="15" t="s">
         <v>506</v>
       </c>
@@ -8957,7 +8957,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="67" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A67" s="15" t="s">
         <v>514</v>
       </c>
@@ -8983,7 +8983,7 @@
       <c r="K67" s="18"/>
       <c r="L67" s="25"/>
     </row>
-    <row r="68" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="68" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A68" s="15" t="s">
         <v>518</v>
       </c>
@@ -9019,7 +9019,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="69" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A69" s="15" t="s">
         <v>526</v>
       </c>
@@ -9053,7 +9053,7 @@
       <c r="K69" s="18"/>
       <c r="L69" s="25"/>
     </row>
-    <row r="70" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="70" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A70" s="15" t="s">
         <v>533</v>
       </c>
@@ -9089,7 +9089,7 @@
       </c>
       <c r="L70" s="25"/>
     </row>
-    <row r="71" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="71" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A71" s="15" t="s">
         <v>540</v>
       </c>
@@ -9125,7 +9125,7 @@
       </c>
       <c r="L71" s="25"/>
     </row>
-    <row r="72" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="72" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A72" s="15" t="s">
         <v>547</v>
       </c>
@@ -9151,7 +9151,7 @@
       <c r="K72" s="18"/>
       <c r="L72" s="25"/>
     </row>
-    <row r="73" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="73" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A73" s="15" t="s">
         <v>550</v>
       </c>
@@ -9187,7 +9187,7 @@
       </c>
       <c r="L73" s="25"/>
     </row>
-    <row r="74" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="74" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A74" s="15" t="s">
         <v>558</v>
       </c>
@@ -9225,7 +9225,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="75" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A75" s="15" t="s">
         <v>565</v>
       </c>
@@ -9259,7 +9259,7 @@
       </c>
       <c r="L75" s="25"/>
     </row>
-    <row r="76" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="76" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A76" s="15" t="s">
         <v>571</v>
       </c>
@@ -9295,7 +9295,7 @@
       </c>
       <c r="L76" s="25"/>
     </row>
-    <row r="77" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="77" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A77" s="15" t="s">
         <v>577</v>
       </c>
@@ -9333,7 +9333,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="78" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A78" s="15" t="s">
         <v>585</v>
       </c>
@@ -9369,7 +9369,7 @@
       </c>
       <c r="L78" s="25"/>
     </row>
-    <row r="79" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="79" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A79" s="15" t="s">
         <v>592</v>
       </c>
@@ -9405,7 +9405,7 @@
       </c>
       <c r="L79" s="25"/>
     </row>
-    <row r="80" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="80" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A80" s="15" t="s">
         <v>600</v>
       </c>
@@ -9441,7 +9441,7 @@
       </c>
       <c r="L80" s="25"/>
     </row>
-    <row r="81" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="81" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A81" s="15" t="s">
         <v>605</v>
       </c>
@@ -9477,7 +9477,7 @@
       </c>
       <c r="L81" s="25"/>
     </row>
-    <row r="82" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="82" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A82" s="15" t="s">
         <v>612</v>
       </c>
@@ -9513,7 +9513,7 @@
       </c>
       <c r="L82" s="25"/>
     </row>
-    <row r="83" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="83" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A83" s="15" t="s">
         <v>618</v>
       </c>
@@ -9549,7 +9549,7 @@
       </c>
       <c r="L83" s="25"/>
     </row>
-    <row r="84" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="84" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A84" s="15" t="s">
         <v>625</v>
       </c>
@@ -9585,7 +9585,7 @@
       </c>
       <c r="L84" s="25"/>
     </row>
-    <row r="85" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="85" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A85" s="15" t="s">
         <v>633</v>
       </c>
@@ -9623,7 +9623,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="86" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="86" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A86" s="15" t="s">
         <v>642</v>
       </c>
@@ -9659,7 +9659,7 @@
       </c>
       <c r="L86" s="25"/>
     </row>
-    <row r="87" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="87" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A87" s="15" t="s">
         <v>650</v>
       </c>
@@ -9695,7 +9695,7 @@
       </c>
       <c r="L87" s="25"/>
     </row>
-    <row r="88" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="88" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A88" s="15" t="s">
         <v>655</v>
       </c>
@@ -9731,7 +9731,7 @@
       </c>
       <c r="L88" s="25"/>
     </row>
-    <row r="89" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="89" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A89" s="15" t="s">
         <v>663</v>
       </c>
@@ -9769,7 +9769,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="90" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="90" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A90" s="15" t="s">
         <v>672</v>
       </c>
@@ -9805,7 +9805,7 @@
       </c>
       <c r="L90" s="25"/>
     </row>
-    <row r="91" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="91" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A91" s="15" t="s">
         <v>679</v>
       </c>
@@ -9831,7 +9831,7 @@
       <c r="K91" s="18"/>
       <c r="L91" s="25"/>
     </row>
-    <row r="92" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="92" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A92" s="15" t="s">
         <v>682</v>
       </c>
@@ -9867,7 +9867,7 @@
       </c>
       <c r="L92" s="25"/>
     </row>
-    <row r="93" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="93" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A93" s="15" t="s">
         <v>689</v>
       </c>
@@ -9903,7 +9903,7 @@
       </c>
       <c r="L93" s="25"/>
     </row>
-    <row r="94" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="94" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A94" s="15" t="s">
         <v>696</v>
       </c>
@@ -9939,7 +9939,7 @@
       </c>
       <c r="L94" s="25"/>
     </row>
-    <row r="95" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="95" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A95" s="15" t="s">
         <v>701</v>
       </c>
@@ -9975,7 +9975,7 @@
       </c>
       <c r="L95" s="25"/>
     </row>
-    <row r="96" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="96" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A96" s="15" t="s">
         <v>709</v>
       </c>
@@ -10013,7 +10013,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="97" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="97" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A97" s="15" t="s">
         <v>717</v>
       </c>
@@ -10051,7 +10051,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="98" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="98" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A98" s="15" t="s">
         <v>726</v>
       </c>
@@ -10087,7 +10087,7 @@
       </c>
       <c r="L98" s="25"/>
     </row>
-    <row r="99" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="99" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A99" s="15" t="s">
         <v>733</v>
       </c>
@@ -10125,7 +10125,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="100" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="100" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A100" s="15" t="s">
         <v>738</v>
       </c>
@@ -10161,7 +10161,7 @@
       </c>
       <c r="L100" s="25"/>
     </row>
-    <row r="101" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="101" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A101" s="15" t="s">
         <v>744</v>
       </c>
@@ -10197,7 +10197,7 @@
       </c>
       <c r="L101" s="25"/>
     </row>
-    <row r="102" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="102" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A102" s="15" t="s">
         <v>751</v>
       </c>
@@ -10235,7 +10235,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="103" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="103" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A103" s="15" t="s">
         <v>760</v>
       </c>
@@ -10269,7 +10269,7 @@
       </c>
       <c r="L103" s="25"/>
     </row>
-    <row r="104" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="104" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A104" s="15" t="s">
         <v>767</v>
       </c>
@@ -10305,7 +10305,7 @@
       </c>
       <c r="L104" s="25"/>
     </row>
-    <row r="105" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="105" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A105" s="15" t="s">
         <v>769</v>
       </c>
@@ -10341,7 +10341,7 @@
       </c>
       <c r="L105" s="25"/>
     </row>
-    <row r="106" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="106" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A106" s="15" t="s">
         <v>780</v>
       </c>
@@ -10377,7 +10377,7 @@
       </c>
       <c r="L106" s="25"/>
     </row>
-    <row r="107" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="107" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A107" s="15" t="s">
         <v>788</v>
       </c>
@@ -10413,7 +10413,7 @@
       </c>
       <c r="L107" s="25"/>
     </row>
-    <row r="108" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="108" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A108" s="15" t="s">
         <v>796</v>
       </c>
@@ -10449,7 +10449,7 @@
       </c>
       <c r="L108" s="25"/>
     </row>
-    <row r="109" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="109" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A109" s="15" t="s">
         <v>804</v>
       </c>
@@ -10485,7 +10485,7 @@
       </c>
       <c r="L109" s="25"/>
     </row>
-    <row r="110" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="110" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A110" s="15" t="s">
         <v>811</v>
       </c>
@@ -10523,7 +10523,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="111" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="111" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A111" s="15" t="s">
         <v>818</v>
       </c>
@@ -10561,7 +10561,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="112" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="112" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A112" s="15" t="s">
         <v>826</v>
       </c>
@@ -10597,7 +10597,7 @@
       </c>
       <c r="L112" s="25"/>
     </row>
-    <row r="113" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="113" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A113" s="15" t="s">
         <v>832</v>
       </c>
@@ -10633,7 +10633,7 @@
       </c>
       <c r="L113" s="25"/>
     </row>
-    <row r="114" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="114" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A114" s="15" t="s">
         <v>839</v>
       </c>
@@ -10669,7 +10669,7 @@
       </c>
       <c r="L114" s="25"/>
     </row>
-    <row r="115" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="115" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A115" s="15" t="s">
         <v>846</v>
       </c>
@@ -10705,7 +10705,7 @@
       </c>
       <c r="L115" s="25"/>
     </row>
-    <row r="116" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="116" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A116" s="15" t="s">
         <v>853</v>
       </c>
@@ -10741,7 +10741,7 @@
       </c>
       <c r="L116" s="25"/>
     </row>
-    <row r="117" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="117" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A117" s="15" t="s">
         <v>858</v>
       </c>
@@ -10777,7 +10777,7 @@
       </c>
       <c r="L117" s="25"/>
     </row>
-    <row r="118" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="118" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A118" s="15" t="s">
         <v>863</v>
       </c>
@@ -10815,7 +10815,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="119" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="119" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A119" s="15" t="s">
         <v>871</v>
       </c>
@@ -10853,7 +10853,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="120" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="120" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A120" s="15" t="s">
         <v>877</v>
       </c>
@@ -10891,7 +10891,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="121" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="121" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A121" s="15" t="s">
         <v>884</v>
       </c>
@@ -10927,7 +10927,7 @@
       </c>
       <c r="L121" s="25"/>
     </row>
-    <row r="122" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="122" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A122" s="15" t="s">
         <v>890</v>
       </c>
@@ -10965,7 +10965,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="123" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="123" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A123" s="15" t="s">
         <v>898</v>
       </c>
@@ -11001,7 +11001,7 @@
       </c>
       <c r="L123" s="25"/>
     </row>
-    <row r="124" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="124" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A124" s="15" t="s">
         <v>905</v>
       </c>
@@ -11037,7 +11037,7 @@
       </c>
       <c r="L124" s="25"/>
     </row>
-    <row r="125" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="125" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A125" s="15" t="s">
         <v>912</v>
       </c>
@@ -11075,7 +11075,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="126" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="126" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A126" s="15" t="s">
         <v>920</v>
       </c>
@@ -11111,7 +11111,7 @@
       </c>
       <c r="L126" s="25"/>
     </row>
-    <row r="127" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="127" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A127" s="15" t="s">
         <v>927</v>
       </c>
@@ -11149,7 +11149,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="128" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="128" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A128" s="15" t="s">
         <v>934</v>
       </c>
@@ -11185,7 +11185,7 @@
       </c>
       <c r="L128" s="25"/>
     </row>
-    <row r="129" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="129" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A129" s="15" t="s">
         <v>941</v>
       </c>
@@ -11223,7 +11223,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="130" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="130" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A130" s="15" t="s">
         <v>657</v>
       </c>
@@ -11261,7 +11261,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="131" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="131" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A131" s="15" t="s">
         <v>956</v>
       </c>
@@ -11297,7 +11297,7 @@
       </c>
       <c r="L131" s="25"/>
     </row>
-    <row r="132" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="132" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A132" s="15" t="s">
         <v>961</v>
       </c>
@@ -11333,7 +11333,7 @@
       </c>
       <c r="L132" s="25"/>
     </row>
-    <row r="133" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="133" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A133" s="15" t="s">
         <v>790</v>
       </c>
@@ -11371,7 +11371,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="134" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="134" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A134" s="15" t="s">
         <v>974</v>
       </c>
@@ -11407,7 +11407,7 @@
       </c>
       <c r="L134" s="25"/>
     </row>
-    <row r="135" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="135" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A135" s="15" t="s">
         <v>981</v>
       </c>
@@ -11443,7 +11443,7 @@
       </c>
       <c r="L135" s="25"/>
     </row>
-    <row r="136" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="136" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A136" s="15" t="s">
         <v>987</v>
       </c>
@@ -11481,7 +11481,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="137" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="137" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A137" s="15" t="s">
         <v>995</v>
       </c>
@@ -11519,7 +11519,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="138" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="138" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A138" s="15" t="s">
         <v>1002</v>
       </c>
@@ -11557,7 +11557,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="139" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="139" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A139" s="15" t="s">
         <v>1011</v>
       </c>
@@ -11595,7 +11595,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="140" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="140" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A140" s="15" t="s">
         <v>1019</v>
       </c>
@@ -11633,7 +11633,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="141" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="141" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A141" s="15" t="s">
         <v>753</v>
       </c>
@@ -11671,7 +11671,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="142" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="142" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A142" s="15" t="s">
         <v>1034</v>
       </c>
@@ -11707,7 +11707,7 @@
       </c>
       <c r="L142" s="25"/>
     </row>
-    <row r="143" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="143" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A143" s="15" t="s">
         <v>1039</v>
       </c>
@@ -11743,7 +11743,7 @@
       </c>
       <c r="L143" s="25"/>
     </row>
-    <row r="144" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="144" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A144" s="15" t="s">
         <v>1046</v>
       </c>
@@ -11779,7 +11779,7 @@
       </c>
       <c r="L144" s="25"/>
     </row>
-    <row r="145" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="145" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A145" s="15" t="s">
         <v>798</v>
       </c>
@@ -11815,7 +11815,7 @@
       </c>
       <c r="L145" s="25"/>
     </row>
-    <row r="146" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="146" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A146" s="15" t="s">
         <v>1061</v>
       </c>
@@ -11853,7 +11853,7 @@
         <v>1068</v>
       </c>
     </row>
-    <row r="147" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="147" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A147" s="15" t="s">
         <v>327</v>
       </c>
@@ -11891,7 +11891,7 @@
         <v>1074</v>
       </c>
     </row>
-    <row r="148" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="148" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A148" s="15" t="s">
         <v>1075</v>
       </c>
@@ -11927,7 +11927,7 @@
       </c>
       <c r="L148" s="25"/>
     </row>
-    <row r="149" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="149" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A149" s="15" t="s">
         <v>1082</v>
       </c>
@@ -11965,7 +11965,7 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="150" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="150" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A150" s="15" t="s">
         <v>215</v>
       </c>
@@ -12001,7 +12001,7 @@
       </c>
       <c r="L150" s="25"/>
     </row>
-    <row r="151" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="151" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A151" s="15" t="s">
         <v>286</v>
       </c>
@@ -12037,7 +12037,7 @@
       </c>
       <c r="L151" s="25"/>
     </row>
-    <row r="152" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="152" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A152" s="15" t="s">
         <v>1102</v>
       </c>
@@ -12073,7 +12073,7 @@
       </c>
       <c r="L152" s="25"/>
     </row>
-    <row r="153" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="153" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A153" s="15" t="s">
         <v>1107</v>
       </c>
@@ -12109,7 +12109,7 @@
       </c>
       <c r="L153" s="25"/>
     </row>
-    <row r="154" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="154" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A154" s="15" t="s">
         <v>1116</v>
       </c>
@@ -12147,7 +12147,7 @@
         <v>1123</v>
       </c>
     </row>
-    <row r="155" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="155" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A155" s="15" t="s">
         <v>1124</v>
       </c>
@@ -12183,7 +12183,7 @@
       </c>
       <c r="L155" s="25"/>
     </row>
-    <row r="156" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="156" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A156" s="15" t="s">
         <v>61</v>
       </c>
@@ -12219,7 +12219,7 @@
       </c>
       <c r="L156" s="25"/>
     </row>
-    <row r="157" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="157" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A157" s="15" t="s">
         <v>1134</v>
       </c>
@@ -12255,7 +12255,7 @@
       </c>
       <c r="L157" s="25"/>
     </row>
-    <row r="158" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="158" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A158" s="15" t="s">
         <v>1141</v>
       </c>
@@ -12289,7 +12289,7 @@
       </c>
       <c r="L158" s="25"/>
     </row>
-    <row r="159" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="159" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A159" s="15" t="s">
         <v>775</v>
       </c>
@@ -12325,7 +12325,7 @@
       </c>
       <c r="L159" s="25"/>
     </row>
-    <row r="160" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="160" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A160" s="15" t="s">
         <v>168</v>
       </c>
@@ -12361,7 +12361,7 @@
       </c>
       <c r="L160" s="25"/>
     </row>
-    <row r="161" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="161" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A161" s="15" t="s">
         <v>1155</v>
       </c>
@@ -12397,7 +12397,7 @@
       </c>
       <c r="L161" s="25"/>
     </row>
-    <row r="162" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="162" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A162" s="15" t="s">
         <v>1161</v>
       </c>
@@ -12435,7 +12435,7 @@
         <v>1167</v>
       </c>
     </row>
-    <row r="163" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="163" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A163" s="15" t="s">
         <v>703</v>
       </c>
@@ -12471,7 +12471,7 @@
       </c>
       <c r="L163" s="25"/>
     </row>
-    <row r="164" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="164" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A164" s="15" t="s">
         <v>1175</v>
       </c>
@@ -12507,7 +12507,7 @@
       </c>
       <c r="L164" s="25"/>
     </row>
-    <row r="165" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="165" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A165" s="15" t="s">
         <v>1182</v>
       </c>
@@ -12543,7 +12543,7 @@
       </c>
       <c r="L165" s="25"/>
     </row>
-    <row r="166" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="166" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A166" s="15" t="s">
         <v>1186</v>
       </c>
@@ -12579,7 +12579,7 @@
       </c>
       <c r="L166" s="25"/>
     </row>
-    <row r="167" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="167" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A167" s="15" t="s">
         <v>1163</v>
       </c>
@@ -12615,7 +12615,7 @@
       </c>
       <c r="L167" s="25"/>
     </row>
-    <row r="168" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="168" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A168" s="15" t="s">
         <v>1198</v>
       </c>
@@ -12653,7 +12653,7 @@
         <v>1205</v>
       </c>
     </row>
-    <row r="169" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="169" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A169" s="15" t="s">
         <v>401</v>
       </c>
@@ -12689,7 +12689,7 @@
       </c>
       <c r="L169" s="25"/>
     </row>
-    <row r="170" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="170" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A170" s="15" t="s">
         <v>1211</v>
       </c>
@@ -12725,7 +12725,7 @@
       </c>
       <c r="L170" s="25"/>
     </row>
-    <row r="171" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="171" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A171" s="15" t="s">
         <v>1217</v>
       </c>
@@ -12761,7 +12761,7 @@
       </c>
       <c r="L171" s="25"/>
     </row>
-    <row r="172" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="172" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A172" s="15" t="s">
         <v>1223</v>
       </c>
@@ -12797,7 +12797,7 @@
       </c>
       <c r="L172" s="25"/>
     </row>
-    <row r="173" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="173" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A173" s="15" t="s">
         <v>719</v>
       </c>
@@ -12835,7 +12835,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="174" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="174" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A174" s="15" t="s">
         <v>1236</v>
       </c>
@@ -12871,7 +12871,7 @@
       </c>
       <c r="L174" s="25"/>
     </row>
-    <row r="175" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="175" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A175" s="15" t="s">
         <v>1243</v>
       </c>
@@ -12907,7 +12907,7 @@
       </c>
       <c r="L175" s="25"/>
     </row>
-    <row r="176" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="176" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A176" s="15" t="s">
         <v>1251</v>
       </c>
@@ -12933,7 +12933,7 @@
       <c r="K176" s="18"/>
       <c r="L176" s="25"/>
     </row>
-    <row r="177" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="177" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A177" s="15" t="s">
         <v>41</v>
       </c>
@@ -12969,7 +12969,7 @@
       </c>
       <c r="L177" s="25"/>
     </row>
-    <row r="178" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="178" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A178" s="15" t="s">
         <v>1262</v>
       </c>
@@ -13005,7 +13005,7 @@
       </c>
       <c r="L178" s="25"/>
     </row>
-    <row r="179" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="179" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A179" s="15" t="s">
         <v>1269</v>
       </c>
@@ -13041,7 +13041,7 @@
       </c>
       <c r="L179" s="25"/>
     </row>
-    <row r="180" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="180" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A180" s="15" t="s">
         <v>1274</v>
       </c>
@@ -13077,7 +13077,7 @@
       </c>
       <c r="L180" s="25"/>
     </row>
-    <row r="181" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="181" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A181" s="15" t="s">
         <v>579</v>
       </c>
@@ -13113,7 +13113,7 @@
       </c>
       <c r="L181" s="25"/>
     </row>
-    <row r="182" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="182" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A182" s="15" t="s">
         <v>1287</v>
       </c>
@@ -13149,7 +13149,7 @@
       </c>
       <c r="L182" s="25"/>
     </row>
-    <row r="183" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="183" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A183" s="15" t="s">
         <v>1295</v>
       </c>
@@ -13187,7 +13187,7 @@
         <v>1303</v>
       </c>
     </row>
-    <row r="184" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="184" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A184" s="15" t="s">
         <v>1304</v>
       </c>
@@ -13223,7 +13223,7 @@
       </c>
       <c r="L184" s="25"/>
     </row>
-    <row r="185" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="185" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A185" s="15" t="s">
         <v>1311</v>
       </c>
@@ -13261,7 +13261,7 @@
         <v>1319</v>
       </c>
     </row>
-    <row r="186" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="186" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A186" s="15" t="s">
         <v>1320</v>
       </c>
@@ -13297,7 +13297,7 @@
       </c>
       <c r="L186" s="25"/>
     </row>
-    <row r="187" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="187" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A187" s="15" t="s">
         <v>1327</v>
       </c>
@@ -13335,7 +13335,7 @@
         <v>1334</v>
       </c>
     </row>
-    <row r="188" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="188" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A188" s="15" t="s">
         <v>1335</v>
       </c>
@@ -13373,7 +13373,7 @@
         <v>1341</v>
       </c>
     </row>
-    <row r="189" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="189" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A189" s="15" t="s">
         <v>1342</v>
       </c>
@@ -13409,7 +13409,7 @@
       </c>
       <c r="L189" s="25"/>
     </row>
-    <row r="190" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="190" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A190" s="15" t="s">
         <v>1348</v>
       </c>
@@ -13445,7 +13445,7 @@
       </c>
       <c r="L190" s="25"/>
     </row>
-    <row r="191" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="191" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A191" s="15" t="s">
         <v>1028</v>
       </c>
@@ -13481,7 +13481,7 @@
       </c>
       <c r="L191" s="25"/>
     </row>
-    <row r="192" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="192" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A192" s="15" t="s">
         <v>1360</v>
       </c>
@@ -13517,7 +13517,7 @@
       </c>
       <c r="L192" s="25"/>
     </row>
-    <row r="193" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="193" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A193" s="15" t="s">
         <v>1366</v>
       </c>
@@ -13553,7 +13553,7 @@
       </c>
       <c r="L193" s="25"/>
     </row>
-    <row r="194" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="194" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A194" s="15" t="s">
         <v>762</v>
       </c>
@@ -13591,7 +13591,7 @@
         <v>1379</v>
       </c>
     </row>
-    <row r="195" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="195" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A195" s="15" t="s">
         <v>1150</v>
       </c>
@@ -13629,7 +13629,7 @@
         <v>1386</v>
       </c>
     </row>
-    <row r="196" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="196" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A196" s="15" t="s">
         <v>1387</v>
       </c>
@@ -13665,7 +13665,7 @@
       </c>
       <c r="L196" s="25"/>
     </row>
-    <row r="197" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="197" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A197" s="15" t="s">
         <v>1393</v>
       </c>
@@ -13701,7 +13701,7 @@
       </c>
       <c r="L197" s="25"/>
     </row>
-    <row r="198" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="198" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A198" s="15" t="s">
         <v>1401</v>
       </c>
@@ -13737,7 +13737,7 @@
       </c>
       <c r="L198" s="25"/>
     </row>
-    <row r="199" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="199" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A199" s="15" t="s">
         <v>1407</v>
       </c>
@@ -13775,7 +13775,7 @@
         <v>1413</v>
       </c>
     </row>
-    <row r="200" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="200" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A200" s="15" t="s">
         <v>1414</v>
       </c>
@@ -13813,7 +13813,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="201" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="201" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A201" s="15" t="s">
         <v>1422</v>
       </c>
@@ -13851,7 +13851,7 @@
         <v>1427</v>
       </c>
     </row>
-    <row r="202" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="202" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A202" s="15" t="s">
         <v>1428</v>
       </c>
@@ -13889,7 +13889,7 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="203" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="203" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A203" s="15" t="s">
         <v>1435</v>
       </c>
@@ -13925,7 +13925,7 @@
       </c>
       <c r="L203" s="25"/>
     </row>
-    <row r="204" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="204" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A204" s="15" t="s">
         <v>1443</v>
       </c>
@@ -13951,7 +13951,7 @@
       <c r="K204" s="18"/>
       <c r="L204" s="25"/>
     </row>
-    <row r="205" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="205" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A205" s="15" t="s">
         <v>1446</v>
       </c>
@@ -13987,7 +13987,7 @@
       </c>
       <c r="L205" s="25"/>
     </row>
-    <row r="206" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="206" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A206" s="15" t="s">
         <v>1453</v>
       </c>
@@ -14013,7 +14013,7 @@
       <c r="K206" s="18"/>
       <c r="L206" s="25"/>
     </row>
-    <row r="207" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="207" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A207" s="15" t="s">
         <v>1322</v>
       </c>
@@ -14049,7 +14049,7 @@
       </c>
       <c r="L207" s="25"/>
     </row>
-    <row r="208" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="208" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A208" s="15" t="s">
         <v>1460</v>
       </c>
@@ -14085,7 +14085,7 @@
       </c>
       <c r="L208" s="25"/>
     </row>
-    <row r="209" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="209" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A209" s="15" t="s">
         <v>1344</v>
       </c>
@@ -14121,7 +14121,7 @@
       </c>
       <c r="L209" s="25"/>
     </row>
-    <row r="210" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="210" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A210" s="15" t="s">
         <v>1282</v>
       </c>
@@ -14157,7 +14157,7 @@
       </c>
       <c r="L210" s="25"/>
     </row>
-    <row r="211" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="211" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A211" s="15" t="s">
         <v>1480</v>
       </c>
@@ -14191,7 +14191,7 @@
       <c r="K211" s="18"/>
       <c r="L211" s="25"/>
     </row>
-    <row r="212" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="212" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A212" s="15" t="s">
         <v>1487</v>
       </c>
@@ -14229,7 +14229,7 @@
         <v>1494</v>
       </c>
     </row>
-    <row r="213" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="213" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A213" s="15" t="s">
         <v>1238</v>
       </c>
@@ -14267,7 +14267,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="214" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="214" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A214" s="15" t="s">
         <v>1501</v>
       </c>
@@ -14303,7 +14303,7 @@
       </c>
       <c r="L214" s="25"/>
     </row>
-    <row r="215" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="215" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A215" s="15" t="s">
         <v>1507</v>
       </c>
@@ -14339,7 +14339,7 @@
       </c>
       <c r="L215" s="25"/>
     </row>
-    <row r="216" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="216" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A216" s="15" t="s">
         <v>1514</v>
       </c>
@@ -14373,7 +14373,7 @@
         <v>1518</v>
       </c>
     </row>
-    <row r="217" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="217" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A217" s="15" t="s">
         <v>1519</v>
       </c>
@@ -14409,7 +14409,7 @@
       </c>
       <c r="L217" s="25"/>
     </row>
-    <row r="218" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="218" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A218" s="15" t="s">
         <v>1527</v>
       </c>
@@ -14445,7 +14445,7 @@
       </c>
       <c r="L218" s="25"/>
     </row>
-    <row r="219" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="219" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A219" s="15" t="s">
         <v>644</v>
       </c>
@@ -14483,7 +14483,7 @@
         <v>1539</v>
       </c>
     </row>
-    <row r="220" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="220" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A220" s="15" t="s">
         <v>1540</v>
       </c>
@@ -14521,7 +14521,7 @@
         <v>1547</v>
       </c>
     </row>
-    <row r="221" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="221" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A221" s="15" t="s">
         <v>1548</v>
       </c>
@@ -14557,7 +14557,7 @@
       </c>
       <c r="L221" s="25"/>
     </row>
-    <row r="222" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="222" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A222" s="15" t="s">
         <v>1403</v>
       </c>
@@ -14593,7 +14593,7 @@
       </c>
       <c r="L222" s="25"/>
     </row>
-    <row r="223" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="223" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A223" s="15" t="s">
         <v>1560</v>
       </c>
@@ -14629,7 +14629,7 @@
       </c>
       <c r="L223" s="25"/>
     </row>
-    <row r="224" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="224" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A224" s="15" t="s">
         <v>1568</v>
       </c>
@@ -14665,7 +14665,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="225" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="225" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A225" s="15" t="s">
         <v>854</v>
       </c>
@@ -14703,7 +14703,7 @@
         <v>1581</v>
       </c>
     </row>
-    <row r="226" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="226" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A226" s="15" t="s">
         <v>185</v>
       </c>
@@ -14741,7 +14741,7 @@
         <v>1588</v>
       </c>
     </row>
-    <row r="227" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="227" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A227" s="15" t="s">
         <v>387</v>
       </c>
@@ -14779,7 +14779,7 @@
         <v>1595</v>
       </c>
     </row>
-    <row r="228" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="228" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A228" s="15" t="s">
         <v>111</v>
       </c>
@@ -14817,7 +14817,7 @@
         <v>1602</v>
       </c>
     </row>
-    <row r="229" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="229" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A229" s="15" t="s">
         <v>1603</v>
       </c>
@@ -14855,7 +14855,7 @@
         <v>1609</v>
       </c>
     </row>
-    <row r="230" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="230" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A230" s="15" t="s">
         <v>1610</v>
       </c>
@@ -14881,7 +14881,7 @@
       <c r="K230" s="25"/>
       <c r="L230" s="25"/>
     </row>
-    <row r="231" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="231" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A231" s="15" t="s">
         <v>1614</v>
       </c>
@@ -14917,7 +14917,7 @@
       </c>
       <c r="L231" s="25"/>
     </row>
-    <row r="232" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="232" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A232" s="15" t="s">
         <v>1618</v>
       </c>
@@ -14955,7 +14955,7 @@
         <v>1624</v>
       </c>
     </row>
-    <row r="233" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="233" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A233" s="15" t="s">
         <v>1625</v>
       </c>
@@ -14991,7 +14991,7 @@
       </c>
       <c r="L233" s="25"/>
     </row>
-    <row r="234" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="234" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A234" s="15" t="s">
         <v>1631</v>
       </c>
@@ -15027,7 +15027,7 @@
       </c>
       <c r="L234" s="25"/>
     </row>
-    <row r="235" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="235" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A235" s="15" t="s">
         <v>1430</v>
       </c>
@@ -15065,7 +15065,7 @@
         <v>1642</v>
       </c>
     </row>
-    <row r="236" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="236" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A236" s="15" t="s">
         <v>1643</v>
       </c>
@@ -15101,7 +15101,7 @@
       </c>
       <c r="L236" s="25"/>
     </row>
-    <row r="237" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="237" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A237" s="15" t="s">
         <v>1648</v>
       </c>
@@ -15137,7 +15137,7 @@
       </c>
       <c r="L237" s="25"/>
     </row>
-    <row r="238" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="238" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A238" s="15" t="s">
         <v>1653</v>
       </c>
@@ -15173,7 +15173,7 @@
       </c>
       <c r="L238" s="25"/>
     </row>
-    <row r="239" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="239" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A239" s="15" t="s">
         <v>1659</v>
       </c>
@@ -15209,7 +15209,7 @@
       </c>
       <c r="L239" s="25"/>
     </row>
-    <row r="240" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="240" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A240" s="15" t="s">
         <v>1245</v>
       </c>
@@ -15243,7 +15243,7 @@
       <c r="K240" s="25"/>
       <c r="L240" s="25"/>
     </row>
-    <row r="241" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="241" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A241" s="15" t="s">
         <v>1668</v>
       </c>
@@ -15275,7 +15275,7 @@
       <c r="K241" s="25"/>
       <c r="L241" s="25"/>
     </row>
-    <row r="242" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="242" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A242" s="15" t="s">
         <v>740</v>
       </c>
@@ -15311,7 +15311,7 @@
       </c>
       <c r="L242" s="25"/>
     </row>
-    <row r="243" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="243" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A243" s="15" t="s">
         <v>1290</v>
       </c>
@@ -15347,7 +15347,7 @@
       </c>
       <c r="L243" s="25"/>
     </row>
-    <row r="244" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="244" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A244" s="15" t="s">
         <v>95</v>
       </c>
@@ -15383,7 +15383,7 @@
       </c>
       <c r="L244" s="25"/>
     </row>
-    <row r="245" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="245" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A245" s="15" t="s">
         <v>1687</v>
       </c>
@@ -15421,7 +15421,7 @@
         <v>1692</v>
       </c>
     </row>
-    <row r="246" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="246" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A246" s="15" t="s">
         <v>635</v>
       </c>
@@ -15457,7 +15457,7 @@
       </c>
       <c r="L246" s="25"/>
     </row>
-    <row r="247" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="247" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A247" s="15" t="s">
         <v>1048</v>
       </c>
@@ -15483,7 +15483,7 @@
       <c r="K247" s="25"/>
       <c r="L247" s="25"/>
     </row>
-    <row r="248" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="248" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A248" s="15" t="s">
         <v>1702</v>
       </c>
@@ -15505,7 +15505,7 @@
       <c r="K248" s="25"/>
       <c r="L248" s="25"/>
     </row>
-    <row r="249" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="249" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A249" s="15" t="s">
         <v>1704</v>
       </c>
@@ -15543,7 +15543,7 @@
         <v>1710</v>
       </c>
     </row>
-    <row r="250" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="250" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A250" s="15" t="s">
         <v>1711</v>
       </c>
@@ -15581,7 +15581,7 @@
         <v>1716</v>
       </c>
     </row>
-    <row r="251" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="251" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A251" s="15" t="s">
         <v>1717</v>
       </c>
@@ -15617,7 +15617,7 @@
       </c>
       <c r="L251" s="25"/>
     </row>
-    <row r="252" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="252" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A252" s="15" t="s">
         <v>1724</v>
       </c>
@@ -15653,7 +15653,7 @@
       </c>
       <c r="L252" s="25"/>
     </row>
-    <row r="253" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="253" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A253" s="15" t="s">
         <v>1730</v>
       </c>
@@ -15687,7 +15687,7 @@
       </c>
       <c r="L253" s="25"/>
     </row>
-    <row r="254" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="254" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A254" s="15" t="s">
         <v>1562</v>
       </c>
@@ -15723,7 +15723,7 @@
       </c>
       <c r="L254" s="25"/>
     </row>
-    <row r="255" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="255" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A255" s="15" t="s">
         <v>1739</v>
       </c>
@@ -15759,7 +15759,7 @@
       </c>
       <c r="L255" s="25"/>
     </row>
-    <row r="256" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="256" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A256" s="15" t="s">
         <v>1612</v>
       </c>
@@ -15795,7 +15795,7 @@
       </c>
       <c r="L256" s="25"/>
     </row>
-    <row r="257" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="257" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A257" s="15" t="s">
         <v>1749</v>
       </c>
@@ -15831,7 +15831,7 @@
       </c>
       <c r="L257" s="25"/>
     </row>
-    <row r="258" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="258" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A258" s="15" t="s">
         <v>1755</v>
       </c>
@@ -15867,7 +15867,7 @@
       </c>
       <c r="L258" s="25"/>
     </row>
-    <row r="259" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="259" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A259" s="15" t="s">
         <v>1761</v>
       </c>
@@ -15905,7 +15905,7 @@
         <v>1767</v>
       </c>
     </row>
-    <row r="260" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="260" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A260" s="15" t="s">
         <v>1362</v>
       </c>
@@ -15941,7 +15941,7 @@
       </c>
       <c r="L260" s="25"/>
     </row>
-    <row r="261" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="261" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A261" s="15" t="s">
         <v>1772</v>
       </c>
@@ -15979,7 +15979,7 @@
         <v>1775</v>
       </c>
     </row>
-    <row r="262" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="262" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A262" s="15" t="s">
         <v>1110</v>
       </c>
@@ -16013,7 +16013,7 @@
       </c>
       <c r="L262" s="25"/>
     </row>
-    <row r="263" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="263" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A263" s="15" t="s">
         <v>620</v>
       </c>
@@ -16051,7 +16051,7 @@
         <v>1787</v>
       </c>
     </row>
-    <row r="264" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="264" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A264" s="15" t="s">
         <v>125</v>
       </c>
@@ -16089,7 +16089,7 @@
         <v>1792</v>
       </c>
     </row>
-    <row r="265" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="265" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A265" s="15" t="s">
         <v>735</v>
       </c>
@@ -16115,7 +16115,7 @@
       <c r="K265" s="25"/>
       <c r="L265" s="25"/>
     </row>
-    <row r="266" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="266" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A266" s="15" t="s">
         <v>1795</v>
       </c>
@@ -16153,7 +16153,7 @@
         <v>1802</v>
       </c>
     </row>
-    <row r="267" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="267" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A267" s="15" t="s">
         <v>1803</v>
       </c>
@@ -16187,7 +16187,7 @@
       </c>
       <c r="L267" s="26"/>
     </row>
-    <row r="268" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="268" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A268" s="15" t="s">
         <v>1808</v>
       </c>
@@ -16225,7 +16225,7 @@
         <v>1815</v>
       </c>
     </row>
-    <row r="269" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="269" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A269" s="15" t="s">
         <v>1350</v>
       </c>
@@ -16261,7 +16261,7 @@
       </c>
       <c r="L269" s="25"/>
     </row>
-    <row r="270" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="270" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A270" s="15" t="s">
         <v>237</v>
       </c>
@@ -16297,7 +16297,7 @@
       </c>
       <c r="L270" s="25"/>
     </row>
-    <row r="271" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="271" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A271" s="15" t="s">
         <v>1826</v>
       </c>
@@ -16333,7 +16333,7 @@
         <v>1831</v>
       </c>
     </row>
-    <row r="272" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="272" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A272" s="15" t="s">
         <v>1832</v>
       </c>
@@ -16367,7 +16367,7 @@
       </c>
       <c r="L272" s="25"/>
     </row>
-    <row r="273" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="273" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A273" s="15" t="s">
         <v>1013</v>
       </c>
@@ -16403,7 +16403,7 @@
       </c>
       <c r="L273" s="25"/>
     </row>
-    <row r="274" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="274" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A274" s="15" t="s">
         <v>1843</v>
       </c>
@@ -16439,7 +16439,7 @@
       </c>
       <c r="L274" s="25"/>
     </row>
-    <row r="275" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="275" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A275" s="15" t="s">
         <v>520</v>
       </c>
@@ -16475,7 +16475,7 @@
       </c>
       <c r="L275" s="25"/>
     </row>
-    <row r="276" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="276" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A276" s="15" t="s">
         <v>1854</v>
       </c>
@@ -16511,7 +16511,7 @@
       </c>
       <c r="L276" s="25"/>
     </row>
-    <row r="277" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="277" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A277" s="15" t="s">
         <v>1468</v>
       </c>
@@ -16547,7 +16547,7 @@
       </c>
       <c r="L277" s="25"/>
     </row>
-    <row r="278" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="278" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A278" s="15" t="s">
         <v>665</v>
       </c>
@@ -16571,7 +16571,7 @@
       <c r="K278" s="18"/>
       <c r="L278" s="25"/>
     </row>
-    <row r="279" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="279" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A279" s="15" t="s">
         <v>1474</v>
       </c>
@@ -16607,7 +16607,7 @@
       </c>
       <c r="L279" s="25"/>
     </row>
-    <row r="280" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="280" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A280" s="15" t="s">
         <v>1868</v>
       </c>
@@ -16643,7 +16643,7 @@
       </c>
       <c r="L280" s="25"/>
     </row>
-    <row r="281" spans="1:12" ht="23.25" x14ac:dyDescent="0.65">
+    <row r="281" spans="1:12" ht="24.6" x14ac:dyDescent="0.85">
       <c r="A281" s="15" t="s">
         <v>1874</v>
       </c>
@@ -16699,32 +16699,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="32" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5546875" customWidth="1"/>
+    <col min="2" max="2" width="22.88671875" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" style="32" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="28.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1893</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="8"/>
       <c r="B2" s="9"/>
       <c r="C2" s="33"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -16741,7 +16741,7 @@
         <v>1884</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -16758,7 +16758,7 @@
         <v>1885</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>2</v>
       </c>
@@ -16775,7 +16775,7 @@
         <v>1887</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>3</v>
       </c>
@@ -16792,7 +16792,7 @@
         <v>1889</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>4</v>
       </c>
@@ -16809,7 +16809,7 @@
         <v>1889</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>5</v>
       </c>
@@ -16826,7 +16826,7 @@
         <v>1889</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>6</v>
       </c>
@@ -16843,35 +16843,35 @@
         <v>1892</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="31"/>
       <c r="C10" s="4"/>
       <c r="D10" s="31"/>
       <c r="E10" s="31"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="31"/>
       <c r="C11" s="4"/>
       <c r="D11" s="31"/>
       <c r="E11" s="31"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="31"/>
       <c r="C12" s="4"/>
       <c r="D12" s="31"/>
       <c r="E12" s="31"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="31"/>
       <c r="C13" s="4"/>
       <c r="D13" s="31"/>
       <c r="E13" s="31"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="31"/>
       <c r="C14" s="4"/>
@@ -16887,26 +16887,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="54.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.44140625" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1899</v>
       </c>
       <c r="C1" s="32"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="8"/>
       <c r="B2" s="9"/>
       <c r="C2" s="33"/>
@@ -16914,7 +16914,7 @@
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -16934,7 +16934,7 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -16954,7 +16954,7 @@
         <v>1903</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -16974,7 +16974,7 @@
         <v>1901</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>2</v>
       </c>
@@ -16990,7 +16990,7 @@
         <v>1901</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>3</v>
       </c>
@@ -17006,7 +17006,7 @@
         <v>1901</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>4</v>
       </c>
@@ -17016,7 +17016,7 @@
       <c r="E8" s="34"/>
       <c r="F8" s="31"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>5</v>
       </c>
@@ -17026,7 +17026,7 @@
       <c r="E9" s="34"/>
       <c r="F9" s="31"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>6</v>
       </c>
@@ -17036,7 +17036,7 @@
       <c r="E10" s="34"/>
       <c r="F10" s="31"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="31"/>
       <c r="C11" s="4"/>
@@ -17044,7 +17044,7 @@
       <c r="E11" s="31"/>
       <c r="F11" s="31"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="31"/>
       <c r="C12" s="4"/>
@@ -17052,7 +17052,7 @@
       <c r="E12" s="31"/>
       <c r="F12" s="31"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="31"/>
       <c r="C13" s="4"/>
@@ -17060,7 +17060,7 @@
       <c r="E13" s="31"/>
       <c r="F13" s="31"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="31"/>
       <c r="C14" s="4"/>
@@ -17068,7 +17068,7 @@
       <c r="E14" s="31"/>
       <c r="F14" s="31"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="31"/>
       <c r="C15" s="4"/>

</xml_diff>